<commit_message>
Modifique diagrama de gant
</commit_message>
<xml_diff>
--- a/doc/proyecto/Diagrama de gant_Vitrigas UNO-A.xlsx
+++ b/doc/proyecto/Diagrama de gant_Vitrigas UNO-A.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Tecnologia - ADSI\Actividades\DAGLINTON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Documentos_Personales\VitriGas_Uno-A\doc\proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97724A0E-5E07-4782-9572-981C77407DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5658532-0EBE-49AA-BDBF-927820AD5C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{92B85D81-18EE-426A-AAB2-B169098CDF5A}"/>
   </bookViews>
@@ -57,76 +57,77 @@
     <t>Trello y Kanban</t>
   </si>
   <si>
+    <t>Entrega de evidencia en la plataforma territorium</t>
+  </si>
+  <si>
+    <t>Taller Identificación, Inventariado y Clasificación de procesos_Bicicletas Colbic</t>
+  </si>
+  <si>
+    <t>Se completo la actividad y se hizo entrega en plataforma territorium</t>
+  </si>
+  <si>
+    <t>Se hicieron correciones y se entrego la evidencia en la plataforma territorium</t>
+  </si>
+  <si>
+    <t>Mapa de procesos (COLBIC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollada y completada </t>
+  </si>
+  <si>
+    <t>Plantillas_Misional y estrategico (COLBIC)</t>
+  </si>
+  <si>
+    <t>Canvas</t>
+  </si>
+  <si>
+    <t>Se dio por terminada la actividad con alguno de los integrantes del grupo, apoyandonos en parte con el material de infotmacion que se nos suministro para completar este proceso</t>
+  </si>
+  <si>
+    <t>Diagrama de gant</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio de diagrama de gant con las actividades </t>
+  </si>
+  <si>
+    <t>Entrega en territorium de evidencia-Diagrama de gant</t>
+  </si>
+  <si>
+    <t>Descripción del software y sus características funcionales y no funcionales</t>
+  </si>
+  <si>
+    <t>Realizacion de la descripcion del software con aportes grupales y evidencia subida a territorium</t>
+  </si>
+  <si>
+    <t>Responsables</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Realizacion de trello y Kanban en herramienta online: </t>
     </r>
     <r>
       <rPr>
-        <u/>
-        <sz val="10"/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>Trello.com</t>
     </r>
-  </si>
-  <si>
-    <t>Entrega de evidencia en la plataforma territorium</t>
-  </si>
-  <si>
-    <t>Taller Identificación, Inventariado y Clasificación de procesos_Bicicletas Colbic</t>
-  </si>
-  <si>
-    <t>Se completo la actividad y se hizo entrega en plataforma territorium</t>
-  </si>
-  <si>
-    <t>Se hicieron correciones y se entrego la evidencia en la plataforma territorium</t>
-  </si>
-  <si>
-    <t>Mapa de procesos (COLBIC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desarrollada y completada </t>
-  </si>
-  <si>
-    <t>Plantillas_Misional y estrategico (COLBIC)</t>
-  </si>
-  <si>
-    <t>Canvas</t>
-  </si>
-  <si>
-    <t>Se dio por terminada la actividad con alguno de los integrantes del grupo, apoyandonos en parte con el material de infotmacion que se nos suministro para completar este proceso</t>
-  </si>
-  <si>
-    <t>Diagrama de gant</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicio de diagrama de gant con las actividades </t>
-  </si>
-  <si>
-    <t>Entrega en territorium de evidencia-Diagrama de gant</t>
-  </si>
-  <si>
-    <t>Descripción del software y sus características funcionales y no funcionales</t>
-  </si>
-  <si>
-    <t>Realizacion de la descripcion del software con aportes grupales y evidencia subida a territorium</t>
-  </si>
-  <si>
-    <t>Responsables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,18 +151,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Arial"/>
     </font>
@@ -169,6 +158,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="16">
@@ -429,16 +425,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -462,9 +450,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -484,10 +469,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -496,34 +481,19 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -534,6 +504,29 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -862,7 +855,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,276 +873,276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="39"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="35"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="4" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="3"/>
+      <c r="N2" s="39"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="5">
+      <c r="A3" s="36"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="1">
         <v>11</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="1">
         <v>12</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="1">
         <v>13</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="1">
         <v>14</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="1">
         <v>18</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="1">
         <v>21</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="1">
         <v>22</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="1">
         <v>26</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="1">
         <v>27</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="2">
         <v>30</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="1">
         <v>2</v>
       </c>
-      <c r="N3" s="7"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="7"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="17" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="22" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="42" t="s">
+      <c r="D11" s="28"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="26" t="s">
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="7"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="28"/>
-      <c r="N12" s="7"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1164,9 +1157,6 @@
       <formula>LEN(TRIM(C2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{CD27B75E-8D80-48F2-9F0D-EB5C626D8018}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>